<commit_message>
remove prefix from final template file names
</commit_message>
<xml_diff>
--- a/raw_excel_oxidative/test_oxidative.xlsx
+++ b/raw_excel_oxidative/test_oxidative.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hava\Documents\R\plater-prep\raw_excel_oxidative\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFC3407D-449D-40D0-9ECA-377952942553}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAFC5096-7683-4DED-BA26-5E34826B7E7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2050-2051-2082" sheetId="1" r:id="rId1"/>
@@ -703,7 +703,7 @@
   <dimension ref="A2:O31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>